<commit_message>
Refactor declaration and history management: Updated styles for declaration layout, removed 'antenne' field from client forms, improved history display with pagination and filtering, and optimized data handling for declarations. Enhanced user experience with better formatting and responsive design adjustments.
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,55 +428,55 @@
         <v>destination</v>
       </c>
       <c r="I1" t="str">
+        <v>itineraire</v>
+      </c>
+      <c r="J1" t="str">
+        <v>driverId</v>
+      </c>
+      <c r="K1" t="str">
+        <v>driverName</v>
+      </c>
+      <c r="L1" t="str">
+        <v>driverCIN</v>
+      </c>
+      <c r="M1" t="str">
+        <v>driverPhone</v>
+      </c>
+      <c r="N1" t="str">
+        <v>vehicleMatricule</v>
+      </c>
+      <c r="O1" t="str">
+        <v>vehicleModel</v>
+      </c>
+      <c r="P1" t="str">
+        <v>convoyeurId</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>convoyeurName</v>
+      </c>
+      <c r="R1" t="str">
+        <v>convoyeurCard</v>
+      </c>
+      <c r="S1" t="str">
+        <v>convoyeurCIN</v>
+      </c>
+      <c r="T1" t="str">
+        <v>convoyeurPhone</v>
+      </c>
+      <c r="U1" t="str">
+        <v>passavantNumber</v>
+      </c>
+      <c r="V1" t="str">
+        <v>passavantExpiry</v>
+      </c>
+      <c r="W1" t="str">
+        <v>bonLivraison</v>
+      </c>
+      <c r="X1" t="str">
         <v>antenne</v>
       </c>
-      <c r="J1" t="str">
-        <v>itineraire</v>
-      </c>
-      <c r="K1" t="str">
-        <v>driverId</v>
-      </c>
-      <c r="L1" t="str">
-        <v>driverName</v>
-      </c>
-      <c r="M1" t="str">
-        <v>driverCIN</v>
-      </c>
-      <c r="N1" t="str">
-        <v>driverPhone</v>
-      </c>
-      <c r="O1" t="str">
-        <v>vehicleMatricule</v>
-      </c>
-      <c r="P1" t="str">
-        <v>vehicleModel</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>convoyeurId</v>
-      </c>
-      <c r="R1" t="str">
-        <v>convoyeurName</v>
-      </c>
-      <c r="S1" t="str">
-        <v>convoyeurCard</v>
-      </c>
-      <c r="T1" t="str">
-        <v>convoyeurCIN</v>
-      </c>
-      <c r="U1" t="str">
-        <v>convoyeurPhone</v>
-      </c>
-      <c r="V1" t="str">
+      <c r="Y1" t="str">
         <v>products</v>
-      </c>
-      <c r="W1" t="str">
-        <v>passavantNumber</v>
-      </c>
-      <c r="X1" t="str">
-        <v>passavantExpiry</v>
-      </c>
-      <c r="Y1" t="str">
-        <v>bonLivraison</v>
       </c>
     </row>
     <row r="2">
@@ -505,54 +505,48 @@
         <v>Warehouse B</v>
       </c>
       <c r="I2" t="str">
-        <v>Antenne 2</v>
-      </c>
-      <c r="J2" t="str">
         <v>Point D, Point E, Point F</v>
       </c>
-      <c r="K2">
+      <c r="J2">
         <v>4</v>
       </c>
+      <c r="K2" t="str">
+        <v>oudra</v>
+      </c>
       <c r="L2" t="str">
-        <v>oudra</v>
+        <v>p3608237</v>
       </c>
       <c r="M2" t="str">
-        <v>p3608237</v>
+        <v>0567233893</v>
       </c>
       <c r="N2" t="str">
-        <v>0567233893</v>
+        <v>sdgas556</v>
       </c>
       <c r="O2" t="str">
-        <v>sdgas556</v>
-      </c>
-      <c r="P2" t="str">
         <v>volvo</v>
       </c>
-      <c r="Q2">
+      <c r="P2">
         <v>2</v>
       </c>
+      <c r="Q2" t="str">
+        <v>Youssef Alaoui</v>
+      </c>
       <c r="R2" t="str">
-        <v>Youssef Alaoui</v>
+        <v>CCE002</v>
       </c>
       <c r="S2" t="str">
-        <v>CCE002</v>
+        <v>YA333444</v>
       </c>
       <c r="T2" t="str">
-        <v>YA333444</v>
+        <v>0656789012</v>
       </c>
       <c r="U2" t="str">
-        <v>0656789012</v>
+        <v>23423432</v>
       </c>
       <c r="V2" t="str">
-        <v>[{"name":"Produit A","quantity":"23","unit":"Kg"}]</v>
+        <v>2025-12-25</v>
       </c>
       <c r="W2" t="str">
-        <v>23423432</v>
-      </c>
-      <c r="X2" t="str">
-        <v>2025-12-25</v>
-      </c>
-      <c r="Y2" t="str">
         <v>43324</v>
       </c>
     </row>
@@ -582,55 +576,52 @@
         <v>ABC Warehouse</v>
       </c>
       <c r="I3" t="str">
+        <v>Route 1, Route 2</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="str">
+        <v>oudra</v>
+      </c>
+      <c r="L3" t="str">
+        <v>p3608237</v>
+      </c>
+      <c r="M3" t="str">
+        <v>0567233893</v>
+      </c>
+      <c r="N3" t="str">
+        <v>sdgas556</v>
+      </c>
+      <c r="O3" t="str">
+        <v>volvo</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>Omar Tazi</v>
+      </c>
+      <c r="R3" t="str">
+        <v>CCE001</v>
+      </c>
+      <c r="S3" t="str">
+        <v>OT111222</v>
+      </c>
+      <c r="T3" t="str">
+        <v>0645678901</v>
+      </c>
+      <c r="U3" t="str">
+        <v>234234</v>
+      </c>
+      <c r="V3" t="str">
+        <v>2025-12-26</v>
+      </c>
+      <c r="W3" t="str">
+        <v>34324</v>
+      </c>
+      <c r="X3" t="str">
         <v>Antenne 3</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Route 1, Route 2</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3" t="str">
-        <v>oudra</v>
-      </c>
-      <c r="M3" t="str">
-        <v>p3608237</v>
-      </c>
-      <c r="N3" t="str">
-        <v>0567233893</v>
-      </c>
-      <c r="O3" t="str">
-        <v>sdgas556</v>
-      </c>
-      <c r="P3" t="str">
-        <v>volvo</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3" t="str">
-        <v>Omar Tazi</v>
-      </c>
-      <c r="S3" t="str">
-        <v>CCE001</v>
-      </c>
-      <c r="T3" t="str">
-        <v>OT111222</v>
-      </c>
-      <c r="U3" t="str">
-        <v>0645678901</v>
-      </c>
-      <c r="V3" t="str">
-        <v>[{"name":"Produit D","quantity":"2","unit":"Tonnes"}]</v>
-      </c>
-      <c r="W3" t="str">
-        <v>234234</v>
-      </c>
-      <c r="X3" t="str">
-        <v>2025-12-26</v>
-      </c>
-      <c r="Y3" t="str">
-        <v>34324</v>
       </c>
     </row>
     <row r="4">
@@ -659,60 +650,131 @@
         <v>ABC Warehouse</v>
       </c>
       <c r="I4" t="str">
-        <v>Antenne 3</v>
-      </c>
-      <c r="J4" t="str">
         <v>Route 1, Route 2</v>
       </c>
-      <c r="K4">
+      <c r="J4">
         <v>1</v>
       </c>
+      <c r="K4" t="str">
+        <v>Ahmed Benali</v>
+      </c>
       <c r="L4" t="str">
-        <v>Ahmed Benali</v>
+        <v>AB123456</v>
       </c>
       <c r="M4" t="str">
-        <v>AB123456</v>
+        <v>0612345678</v>
       </c>
       <c r="N4" t="str">
-        <v>0612345678</v>
+        <v/>
       </c>
       <c r="O4" t="str">
         <v/>
       </c>
-      <c r="P4" t="str">
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>Omar Tazi</v>
+      </c>
+      <c r="R4" t="str">
+        <v>CCE001</v>
+      </c>
+      <c r="S4" t="str">
+        <v>OT111222</v>
+      </c>
+      <c r="T4" t="str">
+        <v>0645678901</v>
+      </c>
+      <c r="U4" t="str">
+        <v>234234</v>
+      </c>
+      <c r="V4" t="str">
+        <v>2025-12-26</v>
+      </c>
+      <c r="W4" t="str">
+        <v>34324</v>
+      </c>
+      <c r="X4" t="str">
+        <v>Antenne 3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1766961828533</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2025-12-28T22:43:48.533Z</v>
+      </c>
+      <c r="C5" t="str">
+        <v>26/2025</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2025-12-19T23:43</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <v>SFI</v>
+      </c>
+      <c r="H5" t="str">
+        <v>SFI Depot</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Point A, Point B, Point C</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Ahmed Benali</v>
+      </c>
+      <c r="L5" t="str">
+        <v>AB123456</v>
+      </c>
+      <c r="M5" t="str">
+        <v>0612345678</v>
+      </c>
+      <c r="N5" t="str">
         <v/>
       </c>
-      <c r="Q4">
+      <c r="O5" t="str">
+        <v/>
+      </c>
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="R4" t="str">
+      <c r="Q5" t="str">
         <v>Omar Tazi</v>
       </c>
-      <c r="S4" t="str">
+      <c r="R5" t="str">
         <v>CCE001</v>
       </c>
-      <c r="T4" t="str">
+      <c r="S5" t="str">
         <v>OT111222</v>
       </c>
-      <c r="U4" t="str">
+      <c r="T5" t="str">
         <v>0645678901</v>
       </c>
-      <c r="V4" t="str">
-        <v>[{"name":"Produit D","quantity":"2","unit":"Tonnes"}]</v>
-      </c>
-      <c r="W4" t="str">
-        <v>234234</v>
-      </c>
-      <c r="X4" t="str">
-        <v>2025-12-26</v>
-      </c>
-      <c r="Y4" t="str">
-        <v>34324</v>
+      <c r="U5" t="str">
+        <v>1221</v>
+      </c>
+      <c r="V5" t="str">
+        <v>2025-12-12</v>
+      </c>
+      <c r="W5" t="str">
+        <v>121212</v>
+      </c>
+      <c r="Y5" t="str">
+        <v>[{"name":"Produit A","quantity":"410","unit":"Kg"}]</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Y4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Y5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>